<commit_message>
Removed email in business name from all reports
</commit_message>
<xml_diff>
--- a/admin/PAYMENT_MADE_REPORT.xlsx
+++ b/admin/PAYMENT_MADE_REPORT.xlsx
@@ -15,18 +15,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
-  <si>
-    <t>PAYMENT MADE REPORT</t>
-  </si>
-  <si>
-    <t>Dance Enterprises, Inc. DBA Arthur Murray Thousand Oaks</t>
-  </si>
-  <si>
-    <t>(12/31/1969 - 01/06/1970)</t>
-  </si>
-  <si>
-    <t>Week # 51</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="54">
+  <si>
+    <t>PAYMENTS MADE REPORT</t>
+  </si>
+  <si>
+    <t>Amto.Robert (Arthur Murray Thousand Oaks, Asansol)</t>
+  </si>
+  <si>
+    <t>(08/10/2025 - 08/23/2025)</t>
   </si>
   <si>
     <t>Payment Date</t>
@@ -78,6 +75,108 @@
   </si>
   <si>
     <t>Teacher3</t>
+  </si>
+  <si>
+    <t>08/20/2025</t>
+  </si>
+  <si>
+    <t>$500.00</t>
+  </si>
+  <si>
+    <t>Wallet Deposit</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Chiara Grieco</t>
+  </si>
+  <si>
+    <t>$2000.00</t>
+  </si>
+  <si>
+    <t>08-15-2025</t>
+  </si>
+  <si>
+    <t>$275.00</t>
+  </si>
+  <si>
+    <t>RC-14192</t>
+  </si>
+  <si>
+    <t>Aar Bagnall</t>
+  </si>
+  <si>
+    <t>Renewal</t>
+  </si>
+  <si>
+    <t>$0.00</t>
+  </si>
+  <si>
+    <t>Edwin Cabrera</t>
+  </si>
+  <si>
+    <t>$250.00</t>
+  </si>
+  <si>
+    <t>RC-14193</t>
+  </si>
+  <si>
+    <t>Robert Melgoza</t>
+  </si>
+  <si>
+    <t>Roumyadeb Karmakar</t>
+  </si>
+  <si>
+    <t>08-18-2025</t>
+  </si>
+  <si>
+    <t>$945.00</t>
+  </si>
+  <si>
+    <t>RC-14195</t>
+  </si>
+  <si>
+    <t>Daisy Ramirez</t>
+  </si>
+  <si>
+    <t>Coach Coach</t>
+  </si>
+  <si>
+    <t>$179.55</t>
+  </si>
+  <si>
+    <t>Refund</t>
+  </si>
+  <si>
+    <t>RC-14194</t>
+  </si>
+  <si>
+    <t>Bronze 2x/Mo Extension</t>
+  </si>
+  <si>
+    <t>09-11-2024</t>
+  </si>
+  <si>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t>$4309.20</t>
+  </si>
+  <si>
+    <t>$4,309.20</t>
+  </si>
+  <si>
+    <t>Caleb Castillo</t>
+  </si>
+  <si>
+    <t>RC-14196</t>
+  </si>
+  <si>
+    <t>$345.45</t>
   </si>
 </sst>
 </file>
@@ -85,7 +184,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -111,6 +210,15 @@
       <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -145,17 +253,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
@@ -166,6 +268,21 @@
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -466,25 +583,31 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="true" style="0"/>
-    <col min="2" max="2" width="12" customWidth="true" style="0"/>
-    <col min="3" max="3" width="12" customWidth="true" style="0"/>
-    <col min="4" max="4" width="12" customWidth="true" style="0"/>
-    <col min="5" max="5" width="12" customWidth="true" style="0"/>
-    <col min="6" max="6" width="12" customWidth="true" style="0"/>
-    <col min="7" max="7" width="12" customWidth="true" style="0"/>
-    <col min="8" max="8" width="12" customWidth="true" style="0"/>
-    <col min="9" max="9" width="12" customWidth="true" style="0"/>
-    <col min="10" max="10" width="12" customWidth="true" style="0"/>
-    <col min="11" max="11" width="12" customWidth="true" style="0"/>
+    <col min="1" max="1" width="13" customWidth="true" style="0"/>
+    <col min="2" max="2" width="13" customWidth="true" style="0"/>
+    <col min="3" max="3" width="13" customWidth="true" style="0"/>
+    <col min="4" max="4" width="13" customWidth="true" style="0"/>
+    <col min="5" max="5" width="13" customWidth="true" style="0"/>
+    <col min="6" max="6" width="13" customWidth="true" style="0"/>
+    <col min="7" max="7" width="13" customWidth="true" style="0"/>
+    <col min="8" max="8" width="13" customWidth="true" style="0"/>
+    <col min="9" max="9" width="13" customWidth="true" style="0"/>
+    <col min="10" max="10" width="13" customWidth="true" style="0"/>
+    <col min="11" max="11" width="13" customWidth="true" style="0"/>
+    <col min="12" max="12" width="13" customWidth="true" style="0"/>
+    <col min="13" max="13" width="13" customWidth="true" style="0"/>
+    <col min="14" max="14" width="10" customWidth="true" style="0"/>
+    <col min="15" max="15" width="13" customWidth="true" style="0"/>
+    <col min="16" max="16" width="13" customWidth="true" style="0"/>
+    <col min="17" max="17" width="13" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" customHeight="1" ht="36">
@@ -493,85 +616,425 @@
       </c>
     </row>
     <row r="2" spans="1:17" customHeight="1" ht="20">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="6" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="N2" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="Q3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="5" t="s">
         <v>20</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="5">
+        <v>1</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="7">
+        <v>1</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="M10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="B11" s="9" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
     <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="I2:M2"/>
-    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="K2:Q2"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
locaiton correction for reports
</commit_message>
<xml_diff>
--- a/admin/PAYMENT_MADE_REPORT.xlsx
+++ b/admin/PAYMENT_MADE_REPORT.xlsx
@@ -15,15 +15,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
   <si>
     <t>PAYMENTS MADE REPORT</t>
   </si>
   <si>
-    <t>Amto.Robert (Arthur Murray Thousand Oaks, Asansol)</t>
-  </si>
-  <si>
-    <t>(08/10/2025 - 08/23/2025)</t>
+    <t>Amto.Robert (Asansol)</t>
+  </si>
+  <si>
+    <t>(08/03/2025 - 08/25/2025)</t>
   </si>
   <si>
     <t>Payment Date</t>
@@ -77,106 +77,7 @@
     <t>Teacher3</t>
   </si>
   <si>
-    <t>08/20/2025</t>
-  </si>
-  <si>
-    <t>$500.00</t>
-  </si>
-  <si>
-    <t>Wallet Deposit</t>
-  </si>
-  <si>
-    <t>Cash</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Chiara Grieco</t>
-  </si>
-  <si>
-    <t>$2000.00</t>
-  </si>
-  <si>
-    <t>08-15-2025</t>
-  </si>
-  <si>
-    <t>$275.00</t>
-  </si>
-  <si>
-    <t>RC-14192</t>
-  </si>
-  <si>
-    <t>Aar Bagnall</t>
-  </si>
-  <si>
-    <t>Renewal</t>
-  </si>
-  <si>
     <t>$0.00</t>
-  </si>
-  <si>
-    <t>Edwin Cabrera</t>
-  </si>
-  <si>
-    <t>$250.00</t>
-  </si>
-  <si>
-    <t>RC-14193</t>
-  </si>
-  <si>
-    <t>Robert Melgoza</t>
-  </si>
-  <si>
-    <t>Roumyadeb Karmakar</t>
-  </si>
-  <si>
-    <t>08-18-2025</t>
-  </si>
-  <si>
-    <t>$945.00</t>
-  </si>
-  <si>
-    <t>RC-14195</t>
-  </si>
-  <si>
-    <t>Daisy Ramirez</t>
-  </si>
-  <si>
-    <t>Coach Coach</t>
-  </si>
-  <si>
-    <t>$179.55</t>
-  </si>
-  <si>
-    <t>Refund</t>
-  </si>
-  <si>
-    <t>RC-14194</t>
-  </si>
-  <si>
-    <t>Bronze 2x/Mo Extension</t>
-  </si>
-  <si>
-    <t>09-11-2024</t>
-  </si>
-  <si>
-    <t>Extension</t>
-  </si>
-  <si>
-    <t>$4309.20</t>
-  </si>
-  <si>
-    <t>$4,309.20</t>
-  </si>
-  <si>
-    <t>Caleb Castillo</t>
-  </si>
-  <si>
-    <t>RC-14196</t>
-  </si>
-  <si>
-    <t>$345.45</t>
   </si>
 </sst>
 </file>
@@ -184,7 +85,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -210,15 +111,6 @@
       <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -253,7 +145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="6">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -268,18 +160,6 @@
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
@@ -583,10 +463,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -692,341 +572,8 @@
       </c>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="5" t="s">
+      <c r="B4" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="5">
-        <v>1</v>
-      </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="P4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q4" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="A5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="5">
-        <v>1</v>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="P5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q5" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="A6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-    </row>
-    <row r="7" spans="1:17">
-      <c r="A7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="O7" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-    </row>
-    <row r="8" spans="1:17">
-      <c r="A8" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" s="5">
-        <v>1</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="N8" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="O8" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-    </row>
-    <row r="9" spans="1:17">
-      <c r="A9" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="N9" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="O9" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-    </row>
-    <row r="10" spans="1:17">
-      <c r="A10" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I10" s="7">
-        <v>1</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="M10" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="N10" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="O10" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-    </row>
-    <row r="11" spans="1:17">
-      <c r="B11" s="9" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
payment made report matching with pdf and excel
</commit_message>
<xml_diff>
--- a/admin/PAYMENT_MADE_REPORT.xlsx
+++ b/admin/PAYMENT_MADE_REPORT.xlsx
@@ -15,15 +15,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="116">
   <si>
     <t>PAYMENTS MADE REPORT</t>
   </si>
   <si>
-    <t>Amto.Robert (Asansol)</t>
-  </si>
-  <si>
-    <t>(08/03/2025 - 08/25/2025)</t>
+    <t>Amto.Robert (Arthur Murray Thousand Oaks, Asansol)</t>
+  </si>
+  <si>
+    <t>(05/01/2025 - 09/04/2025)</t>
   </si>
   <si>
     <t>Payment Date</t>
@@ -77,7 +77,292 @@
     <t>Teacher3</t>
   </si>
   <si>
+    <t>05-22-2025</t>
+  </si>
+  <si>
+    <t>$15000.00</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>RC-14177</t>
+  </si>
+  <si>
+    <t>Aaron Frye</t>
+  </si>
+  <si>
+    <t>04-28-2025</t>
+  </si>
+  <si>
+    <t>Miscellanious service</t>
+  </si>
+  <si>
     <t>$0.00</t>
+  </si>
+  <si>
+    <t>Edwin Cabrera</t>
+  </si>
+  <si>
+    <t>Time Exchange</t>
+  </si>
+  <si>
+    <t>06-04-2025</t>
+  </si>
+  <si>
+    <t>RC-14178</t>
+  </si>
+  <si>
+    <t>Aar Bagnall</t>
+  </si>
+  <si>
+    <t>Roumyadeb Karmakar</t>
+  </si>
+  <si>
+    <t>$180.00</t>
+  </si>
+  <si>
+    <t>RC-14179</t>
+  </si>
+  <si>
+    <t>Aaron Alcantara</t>
+  </si>
+  <si>
+    <t>Robert Melgoza</t>
+  </si>
+  <si>
+    <t>$380.00</t>
+  </si>
+  <si>
+    <t>RC-14180</t>
+  </si>
+  <si>
+    <t>Akethea Clarke</t>
+  </si>
+  <si>
+    <t>Pre original</t>
+  </si>
+  <si>
+    <t>Daisy Ramirez</t>
+  </si>
+  <si>
+    <t>$1000.00</t>
+  </si>
+  <si>
+    <t>RC-14181</t>
+  </si>
+  <si>
+    <t>Aaron Bagnall</t>
+  </si>
+  <si>
+    <t>$2500.00</t>
+  </si>
+  <si>
+    <t>RC-14182</t>
+  </si>
+  <si>
+    <t>Original</t>
+  </si>
+  <si>
+    <t>RC-14183</t>
+  </si>
+  <si>
+    <t>Anna Tripp</t>
+  </si>
+  <si>
+    <t>06-23-2025</t>
+  </si>
+  <si>
+    <t>$500.00</t>
+  </si>
+  <si>
+    <t>RC-14184</t>
+  </si>
+  <si>
+    <t>Coach Coach</t>
+  </si>
+  <si>
+    <t>07-31-2025</t>
+  </si>
+  <si>
+    <t>$160.65</t>
+  </si>
+  <si>
+    <t>RC-14185</t>
+  </si>
+  <si>
+    <t>Carol Henry</t>
+  </si>
+  <si>
+    <t>Bronze 5x/Mo Extension</t>
+  </si>
+  <si>
+    <t>12-03-2024</t>
+  </si>
+  <si>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t>$9639.00</t>
+  </si>
+  <si>
+    <t>$9,478.35</t>
+  </si>
+  <si>
+    <t>Caleb Castillo</t>
+  </si>
+  <si>
+    <t>08-01-2025</t>
+  </si>
+  <si>
+    <t>$510.30</t>
+  </si>
+  <si>
+    <t>RC-14186</t>
+  </si>
+  <si>
+    <t>Steve Bowerman</t>
+  </si>
+  <si>
+    <t>Bronze 3x/Mo Extension</t>
+  </si>
+  <si>
+    <t>08-15-2024</t>
+  </si>
+  <si>
+    <t>$6123.60</t>
+  </si>
+  <si>
+    <t>$5,613.30</t>
+  </si>
+  <si>
+    <t>RC-14187</t>
+  </si>
+  <si>
+    <t>$179.55</t>
+  </si>
+  <si>
+    <t>RC-14188</t>
+  </si>
+  <si>
+    <t>Emily Hare</t>
+  </si>
+  <si>
+    <t>2x/Mo Renewal</t>
+  </si>
+  <si>
+    <t>12-12-2024</t>
+  </si>
+  <si>
+    <t>Renewal</t>
+  </si>
+  <si>
+    <t>$4309.20</t>
+  </si>
+  <si>
+    <t>$4,129.65</t>
+  </si>
+  <si>
+    <t>RC-14189</t>
+  </si>
+  <si>
+    <t>$359.10</t>
+  </si>
+  <si>
+    <t>RC-14190</t>
+  </si>
+  <si>
+    <t>Chiara Grieco</t>
+  </si>
+  <si>
+    <t>Bronze 2x/Mo Extension</t>
+  </si>
+  <si>
+    <t>09-11-2024</t>
+  </si>
+  <si>
+    <t>$3,950.10</t>
+  </si>
+  <si>
+    <t>$680.40</t>
+  </si>
+  <si>
+    <t>RC-14191</t>
+  </si>
+  <si>
+    <t>Roger Dewames</t>
+  </si>
+  <si>
+    <t>4x/Mo Renewal</t>
+  </si>
+  <si>
+    <t>09-03-2024</t>
+  </si>
+  <si>
+    <t>$8164.80</t>
+  </si>
+  <si>
+    <t>$7,484.40</t>
+  </si>
+  <si>
+    <t>08-15-2025</t>
+  </si>
+  <si>
+    <t>$275.00</t>
+  </si>
+  <si>
+    <t>RC-14192</t>
+  </si>
+  <si>
+    <t>$250.00</t>
+  </si>
+  <si>
+    <t>RC-14193</t>
+  </si>
+  <si>
+    <t>08-18-2025</t>
+  </si>
+  <si>
+    <t>$945.00</t>
+  </si>
+  <si>
+    <t>RC-14195</t>
+  </si>
+  <si>
+    <t>08-27-2025</t>
+  </si>
+  <si>
+    <t>Manual Payment</t>
+  </si>
+  <si>
+    <t>Wallet</t>
+  </si>
+  <si>
+    <t>09-02-2025</t>
+  </si>
+  <si>
+    <t>RC-14197</t>
+  </si>
+  <si>
+    <t>NEW</t>
+  </si>
+  <si>
+    <t>Refund</t>
+  </si>
+  <si>
+    <t>RC-14194</t>
+  </si>
+  <si>
+    <t>$4,309.20</t>
+  </si>
+  <si>
+    <t>RC-14196</t>
+  </si>
+  <si>
+    <t>$39,976.75</t>
   </si>
 </sst>
 </file>
@@ -85,7 +370,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -111,6 +396,15 @@
       <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -145,7 +439,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -160,6 +454,18 @@
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
@@ -463,10 +769,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -572,8 +878,1024 @@
       </c>
     </row>
     <row r="4" spans="1:17">
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="5" t="s">
         <v>20</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="5">
+        <v>1</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="5">
+        <v>1</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="5">
+        <v>2</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="5">
+        <v>3</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" s="5">
+        <v>55</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" s="5">
+        <v>2</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="5">
+        <v>1</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O12" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O16" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="O17" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="M18" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="N18" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="L20" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="O20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="I21" s="5">
+        <v>1</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N21" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="O21" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="5">
+        <v>1</v>
+      </c>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="I22" s="5">
+        <v>1</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L22" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="M22" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O22" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="L23" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="M23" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N23" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="O23" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="L24" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="M24" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="N24" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="O24" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="I25" s="7">
+        <v>1</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="L25" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="M25" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="N25" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="O25" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="B26" s="9" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>